<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T01:46:20.685Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -561,7 +561,7 @@
         <v>COOKING</v>
       </c>
       <c r="I4" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J4" t="str">
         <v>2026-01-20</v>
@@ -832,10 +832,10 @@
         <v>525</v>
       </c>
       <c r="F3">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="G3">
-        <v>285</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T02:14:07.600Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -558,7 +558,7 @@
         <v>120</v>
       </c>
       <c r="H4" t="str">
-        <v>COOKING</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T02:14:11.536Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -558,7 +558,7 @@
         <v>120</v>
       </c>
       <c r="H4" t="str">
-        <v>DELIVERED</v>
+        <v>READY</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T02:24:50.521Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -470,7 +470,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>READY</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T02:48:54.674Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -690,7 +690,7 @@
         <v>105</v>
       </c>
       <c r="H7" t="str">
-        <v>READY</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T02:48:58.229Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -558,7 +558,7 @@
         <v>120</v>
       </c>
       <c r="H4" t="str">
-        <v>READY</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T04:28:18.973Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -473,7 +473,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
@@ -809,10 +809,10 @@
         <v>30</v>
       </c>
       <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
         <v>0</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T04:28:32.390Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -561,7 +561,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J4" t="str">
         <v>2026-01-20</v>
@@ -832,10 +832,10 @@
         <v>525</v>
       </c>
       <c r="F3">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="G3">
-        <v>405</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T05:33:38.061Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,37 +449,37 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D2" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E2" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G2">
         <v>20</v>
       </c>
-      <c r="B2" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D2" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E2" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C3" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D3" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E3" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G3">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>DELIVERED</v>
@@ -520,10 +520,10 @@
         <v>PAID</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,22 +537,22 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C4" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D4" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E4" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F4" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G4">
         <v>120</v>
@@ -564,10 +564,10 @@
         <v>PAID</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K4" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,34 +581,34 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C5" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D5" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E5" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G5">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H5" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I5" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
         <v>08:00</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C6" t="str">
         <v>Prajakta Patil</v>
@@ -640,10 +640,10 @@
         <v>779868817</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G6">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,7 +652,7 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K6" t="str">
         <v>08:00</v>
@@ -669,10 +669,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C7" t="str">
         <v>Prajakta Patil</v>
@@ -690,19 +690,19 @@
         <v>105</v>
       </c>
       <c r="H7" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K7" t="str">
         <v>08:00</v>
       </c>
       <c r="L7" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M7" t="str">
         <v/>
@@ -713,51 +713,95 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C8" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D8" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E8" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G8">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H8" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I8" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J8" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K8" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D9" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E9" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G9">
+        <v>600</v>
+      </c>
+      <c r="H9" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I9" t="str">
         <v>PAID</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J9" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K9" t="str">
         <v>00:30</v>
       </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -797,7 +841,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -806,13 +850,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>30</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T05:33:52.632Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -470,7 +470,7 @@
         <v>20</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T05:33:57.072Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -473,7 +473,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
@@ -853,10 +853,10 @@
         <v>50</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T09:42:17.125Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -737,7 +737,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I8" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J8" t="str">
         <v>2026-01-20</v>
@@ -876,10 +876,10 @@
         <v>525</v>
       </c>
       <c r="F3">
-        <v>240</v>
+        <v>345</v>
       </c>
       <c r="G3">
-        <v>285</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T11:13:40.585Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,37 +449,37 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C2" t="str">
         <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E2" t="str">
         <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E3" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G3">
         <v>20</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D3" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E3" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>DELIVERED</v>
@@ -523,7 +523,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C4" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D4" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E4" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G4">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>DELIVERED</v>
@@ -564,10 +564,10 @@
         <v>PAID</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,22 +581,22 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C5" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D5" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E5" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F5" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -608,10 +608,10 @@
         <v>PAID</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K5" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,34 +625,34 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C6" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D6" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E6" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G6">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H6" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I6" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
         <v>08:00</v>
@@ -669,10 +669,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C7" t="str">
         <v>Prajakta Patil</v>
@@ -684,10 +684,10 @@
         <v>779868817</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G7">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,7 +696,7 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K7" t="str">
         <v>08:00</v>
@@ -713,10 +713,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C8" t="str">
         <v>Prajakta Patil</v>
@@ -734,19 +734,19 @@
         <v>105</v>
       </c>
       <c r="H8" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I8" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K8" t="str">
         <v>08:00</v>
       </c>
       <c r="L8" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C9" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D9" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E9" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G9">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H9" t="str">
         <v>DELIVERED</v>
@@ -784,24 +784,68 @@
         <v>PAID</v>
       </c>
       <c r="J9" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K9" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D10" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E10" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G10">
+        <v>600</v>
+      </c>
+      <c r="H10" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I10" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J10" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K10" t="str">
         <v>00:30</v>
       </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-      <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -841,7 +885,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -850,13 +894,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T11:14:12.131Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -470,7 +470,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T12:17:31.770Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,37 +449,37 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D2" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,37 +493,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C3" t="str">
         <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E3" t="str">
         <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D4" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E4" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G4">
         <v>20</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D4" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E4" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>DELIVERED</v>
@@ -567,7 +567,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C5" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D5" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E5" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G5">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
@@ -608,10 +608,10 @@
         <v>PAID</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,22 +625,22 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C6" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D6" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E6" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F6" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G6">
         <v>120</v>
@@ -652,10 +652,10 @@
         <v>PAID</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K6" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,34 +669,34 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C7" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D7" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E7" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G7">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H7" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I7" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K7" t="str">
         <v>08:00</v>
@@ -713,10 +713,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C8" t="str">
         <v>Prajakta Patil</v>
@@ -728,10 +728,10 @@
         <v>779868817</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G8">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,7 +740,7 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K8" t="str">
         <v>08:00</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C9" t="str">
         <v>Prajakta Patil</v>
@@ -778,19 +778,19 @@
         <v>105</v>
       </c>
       <c r="H9" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I9" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K9" t="str">
         <v>08:00</v>
       </c>
       <c r="L9" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C10" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D10" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E10" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G10">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H10" t="str">
         <v>DELIVERED</v>
@@ -828,24 +828,68 @@
         <v>PAID</v>
       </c>
       <c r="J10" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K10" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D11" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E11" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G11">
+        <v>600</v>
+      </c>
+      <c r="H11" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I11" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J11" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K10" t="str">
+      <c r="K11" t="str">
         <v>00:30</v>
       </c>
-      <c r="L10" t="str">
-        <v/>
-      </c>
-      <c r="M10" t="str">
-        <v/>
-      </c>
-      <c r="N10" t="str">
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -885,7 +929,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -894,13 +938,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>80</v>
+        <v>260</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T15:03:47.593Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C2" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D2" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E2" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F2" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,13 +476,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,37 +493,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D3" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H3" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K3" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,37 +537,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C4" t="str">
         <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E4" t="str">
         <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J4" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D5" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E5" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G5">
         <v>20</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D5" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E5" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
@@ -611,7 +611,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C6" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D6" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E6" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F6" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G6">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
@@ -652,10 +652,10 @@
         <v>PAID</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,22 +669,22 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C7" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D7" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E7" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F7" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G7">
         <v>120</v>
@@ -696,10 +696,10 @@
         <v>PAID</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K7" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,34 +713,34 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C8" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D8" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E8" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G8">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H8" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I8" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K8" t="str">
         <v>08:00</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C9" t="str">
         <v>Prajakta Patil</v>
@@ -772,10 +772,10 @@
         <v>779868817</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G9">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -784,7 +784,7 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K9" t="str">
         <v>08:00</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C10" t="str">
         <v>Prajakta Patil</v>
@@ -822,19 +822,19 @@
         <v>105</v>
       </c>
       <c r="H10" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I10" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K10" t="str">
         <v>08:00</v>
       </c>
       <c r="L10" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C11" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D11" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E11" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F11" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G11">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H11" t="str">
         <v>DELIVERED</v>
@@ -872,24 +872,68 @@
         <v>PAID</v>
       </c>
       <c r="J11" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K11" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D12" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E12" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G12">
+        <v>600</v>
+      </c>
+      <c r="H12" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I12" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J12" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K11" t="str">
+      <c r="K12" t="str">
         <v>00:30</v>
       </c>
-      <c r="L11" t="str">
-        <v/>
-      </c>
-      <c r="M11" t="str">
-        <v/>
-      </c>
-      <c r="N11" t="str">
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -929,7 +973,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -938,13 +982,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
       <c r="G2">
-        <v>210</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T15:05:12.391Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,19 +449,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 15:03</v>
+        <v>2026-01-20 15:05</v>
       </c>
       <c r="C2" t="str">
-        <v>Udita Roy</v>
+        <v>Indrani Karmakar</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1603</v>
+        <v>A-1903</v>
       </c>
       <c r="E2" t="str">
-        <v>7061856166</v>
+        <v>7030961520</v>
       </c>
       <c r="F2" t="str">
         <v>Appe Chutney x1</v>
@@ -479,7 +479,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v>09:30</v>
+        <v>09:00</v>
       </c>
       <c r="L2" t="str">
         <v>Less spicy. Flavourful</v>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C3" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D3" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E3" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F3" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G3">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,13 +520,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -537,37 +537,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D4" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H4" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K4" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,37 +581,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C5" t="str">
         <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E5" t="str">
         <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I5" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J5" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D6" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E6" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G6">
         <v>20</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D6" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E6" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
@@ -655,7 +655,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C7" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D7" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E7" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F7" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G7">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>DELIVERED</v>
@@ -696,10 +696,10 @@
         <v>PAID</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K7" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,22 +713,22 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C8" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D8" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E8" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F8" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G8">
         <v>120</v>
@@ -740,10 +740,10 @@
         <v>PAID</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K8" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,34 +757,34 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C9" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D9" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E9" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G9">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H9" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I9" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K9" t="str">
         <v>08:00</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C10" t="str">
         <v>Prajakta Patil</v>
@@ -816,10 +816,10 @@
         <v>779868817</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G10">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -828,7 +828,7 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K10" t="str">
         <v>08:00</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C11" t="str">
         <v>Prajakta Patil</v>
@@ -866,19 +866,19 @@
         <v>105</v>
       </c>
       <c r="H11" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I11" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K11" t="str">
         <v>08:00</v>
       </c>
       <c r="L11" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C12" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D12" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E12" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F12" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G12">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H12" t="str">
         <v>DELIVERED</v>
@@ -916,24 +916,68 @@
         <v>PAID</v>
       </c>
       <c r="J12" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K12" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D13" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E13" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G13">
+        <v>600</v>
+      </c>
+      <c r="H13" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I13" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J13" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K12" t="str">
+      <c r="K13" t="str">
         <v>00:30</v>
       </c>
-      <c r="L12" t="str">
-        <v/>
-      </c>
-      <c r="M12" t="str">
-        <v/>
-      </c>
-      <c r="N12" t="str">
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -973,7 +1017,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -982,13 +1026,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
       <c r="G2">
-        <v>270</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T16:18:01.482Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -473,7 +473,7 @@
         <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-21</v>
@@ -517,7 +517,7 @@
         <v>NEW</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-21</v>
@@ -1029,10 +1029,10 @@
         <v>380</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="G2">
-        <v>330</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-20.xlsx - 2026-01-20T17:36:50.871Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,40 +449,40 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 15:05</v>
+        <v>2026-01-20 17:36</v>
       </c>
       <c r="C2" t="str">
-        <v>Indrani Karmakar</v>
+        <v>Priyanka Patil</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1903</v>
+        <v>A-1605</v>
       </c>
       <c r="E2" t="str">
-        <v>7030961520</v>
+        <v>9867003224</v>
       </c>
       <c r="F2" t="str">
-        <v>Appe Chutney x1</v>
+        <v>Appe Chutney x2</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v>09:00</v>
+        <v>09:15</v>
       </c>
       <c r="L2" t="str">
-        <v>Less spicy. Flavourful</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,19 +493,19 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 15:03</v>
+        <v>2026-01-20 15:05</v>
       </c>
       <c r="C3" t="str">
-        <v>Udita Roy</v>
+        <v>Indrani Karmakar</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1603</v>
+        <v>A-1903</v>
       </c>
       <c r="E3" t="str">
-        <v>7061856166</v>
+        <v>7030961520</v>
       </c>
       <c r="F3" t="str">
         <v>Appe Chutney x1</v>
@@ -523,7 +523,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
-        <v>09:30</v>
+        <v>09:00</v>
       </c>
       <c r="L3" t="str">
         <v>Less spicy. Flavourful</v>
@@ -537,40 +537,40 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C4" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D4" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E4" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F4" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G4">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
       </c>
       <c r="I4" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -581,37 +581,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D5" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H5" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K5" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,37 +625,37 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C6" t="str">
         <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E6" t="str">
         <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I6" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J6" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
+        <v>21</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D7" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E7" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G7">
         <v>20</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D7" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E7" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>DELIVERED</v>
@@ -699,7 +699,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K7" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C8" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D8" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E8" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F8" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G8">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>DELIVERED</v>
@@ -740,10 +740,10 @@
         <v>PAID</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K8" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,22 +757,22 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C9" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D9" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E9" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F9" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G9">
         <v>120</v>
@@ -784,10 +784,10 @@
         <v>PAID</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K9" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,34 +801,34 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C10" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D10" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E10" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G10">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H10" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I10" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K10" t="str">
         <v>08:00</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C11" t="str">
         <v>Prajakta Patil</v>
@@ -860,10 +860,10 @@
         <v>779868817</v>
       </c>
       <c r="F11" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G11">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -872,7 +872,7 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K11" t="str">
         <v>08:00</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C12" t="str">
         <v>Prajakta Patil</v>
@@ -910,19 +910,19 @@
         <v>105</v>
       </c>
       <c r="H12" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I12" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J12" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K12" t="str">
         <v>08:00</v>
       </c>
       <c r="L12" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C13" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D13" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E13" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F13" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G13">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H13" t="str">
         <v>DELIVERED</v>
@@ -960,24 +960,68 @@
         <v>PAID</v>
       </c>
       <c r="J13" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K13" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D14" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E14" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G14">
+        <v>600</v>
+      </c>
+      <c r="H14" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I14" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J14" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K13" t="str">
+      <c r="K14" t="str">
         <v>00:30</v>
       </c>
-      <c r="L13" t="str">
-        <v/>
-      </c>
-      <c r="M13" t="str">
-        <v/>
-      </c>
-      <c r="N13" t="str">
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N14"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1017,7 +1061,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1026,13 +1070,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>380</v>
+        <v>500</v>
       </c>
       <c r="F2">
         <v>170</v>
       </c>
       <c r="G2">
-        <v>210</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">

</xml_diff>